<commit_message>
Examples from 11 to 19 added
</commit_message>
<xml_diff>
--- a/AMC_examples_data/AMC_examples_data_ex10.xlsx
+++ b/AMC_examples_data/AMC_examples_data_ex10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\AMC_examples_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88578F6B-DB89-4F7F-A168-8AD24E2E548F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A6AB53-0237-4518-B45C-F9321DBC0F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
+    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" xr2:uid="{FFF8BB56-E23A-426B-9D6C-DA86724C81B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>frame_h</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>(si, non mi sono sbagliato, il secondo e il terzo candidato sono identici)</t>
+  </si>
+  <si>
+    <t>INCONSISTENTE</t>
+  </si>
+  <si>
+    <t>ESEMPIO INCONSISTENTE</t>
   </si>
 </sst>
 </file>
@@ -113,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,8 +145,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -449,22 +462,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F28914-79CE-4C5A-92B2-E41C9BEF8F7E}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="50" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" customWidth="1"/>
     <col min="11" max="11" width="41.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -636,6 +654,11 @@
       </c>
       <c r="M6" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>